<commit_message>
Changes in Zee5 and SunNxt
</commit_message>
<xml_diff>
--- a/appium/Results/ExcelSheetsFolder/07072025/ExcelResults.xlsx
+++ b/appium/Results/ExcelSheetsFolder/07072025/ExcelResults.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7C17C0A6-766F-4B74-985E-A7CDAF7308B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{655B32FE-0074-4AEB-937D-2D03D71E90BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="07072025" sheetId="1" r:id="rId1"/>
     <sheet name="JSTV210" sheetId="2" r:id="rId2"/>
-    <sheet name="JSTV220" r:id="rId6" sheetId="3"/>
-    <sheet name="JHSC200" r:id="rId7" sheetId="4"/>
+    <sheet name="JHSC200" sheetId="4" r:id="rId3"/>
+    <sheet name="JSTV220" r:id="rId7" sheetId="5"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1:J16"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="56">
   <si>
     <t>DeviceName</t>
   </si>
@@ -180,16 +180,13 @@
     <t>sonyliv_3.4.49</t>
   </si>
   <si>
+    <t>NA NA</t>
+  </si>
+  <si>
+    <t>src_fmt = invaild</t>
+  </si>
+  <si>
     <t>JSTV220_00.00.72.40.CBSPP</t>
-  </si>
-  <si>
-    <t>zee5_5.65.1</t>
-  </si>
-  <si>
-    <t>src_fmt = invalid</t>
-  </si>
-  <si>
-    <t>NA NA</t>
   </si>
 </sst>
 </file>
@@ -1485,11 +1482,913 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.1796875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.08984375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.08984375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.453125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.08984375"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.96484375"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.7265625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.1796875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.08984375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.08984375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.453125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.08984375"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s" s="0">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F21" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.59375"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="18.17578125"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="28.09765625"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.1171875"/>
@@ -1497,287 +2396,6 @@
     <col min="6" max="6" bestFit="true" customWidth="true" width="14.10546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="F11" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E12" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="F12" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.59375"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.65234375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.12109375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.1171875"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.1875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.10546875"/>
-  </cols>
-  <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
         <v>0</v>
@@ -1800,33 +2418,33 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>10</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>9</v>
@@ -1835,21 +2453,21 @@
         <v>10</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>10</v>
@@ -1860,53 +2478,53 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>11</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>14</v>
@@ -1915,108 +2533,87 @@
         <v>10</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s" s="0">
         <v>14</v>
       </c>
       <c r="E8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="F8" t="s" s="0">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.7265625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.65234375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.17578125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.1171875"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.11328125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.10546875"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>11</v>
+      <c r="B9" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>